<commit_message>
extend and categorise keyword list further
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ee3ec44abf2629a/Dokumente/Privat/Uni/HWR/SHK/AIRI_Analyser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnandarL\source\repos\SHK-AIRI-Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="11_9DEFDF395517B64B77C7F2E85816A4F5402FF0BF" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CDDD2DED-BDC3-441A-B689-CC994AB40EFA}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="3110" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="3108" windowWidth="28800" windowHeight="15456"/>
   </bookViews>
   <sheets>
     <sheet name="First Draft" sheetId="1" r:id="rId1"/>
     <sheet name="SchmidtLampe" sheetId="2" r:id="rId2"/>
+    <sheet name="WolfVitale" sheetId="4" r:id="rId3"/>
+    <sheet name="Anandarajah" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="296">
   <si>
     <t>Digitalisierung</t>
   </si>
@@ -348,12 +349,573 @@
   </si>
   <si>
     <t>strong AI</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Consulting &amp; Optimising</t>
+  </si>
+  <si>
+    <t>Smart IoT</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Quality Control</t>
+  </si>
+  <si>
+    <t>Inspections</t>
+  </si>
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>Malware-Detection</t>
+  </si>
+  <si>
+    <t>Root-Cause-Failure Analysis</t>
+  </si>
+  <si>
+    <t>Predictive Maintenance</t>
+  </si>
+  <si>
+    <t>Risk Scoring</t>
+  </si>
+  <si>
+    <t>Customer Behaviour</t>
+  </si>
+  <si>
+    <t>Market Research</t>
+  </si>
+  <si>
+    <t>Prognoses</t>
+  </si>
+  <si>
+    <t>Rapid Alert Systems</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Predictive Content</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Affective Computing</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Research &amp; Development</t>
+  </si>
+  <si>
+    <t>Knowledge Management</t>
+  </si>
+  <si>
+    <t>Advertising, PR</t>
+  </si>
+  <si>
+    <t>Intelligent sensors</t>
+  </si>
+  <si>
+    <t>Networked Devices</t>
+  </si>
+  <si>
+    <t>Digital Assistance Systems</t>
+  </si>
+  <si>
+    <t>Kognitive Systems</t>
+  </si>
+  <si>
+    <t>Customer Relations</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>Workflow-Management</t>
+  </si>
+  <si>
+    <t>Operations Facilities &amp; Fleet Management</t>
+  </si>
+  <si>
+    <t>Purchasing, Logistics, Supply Chain</t>
+  </si>
+  <si>
+    <t>Finance &amp; Accounting</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Provisioning</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>IT &amp; System Administration</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>biocybernetics</t>
+  </si>
+  <si>
+    <t>design and control</t>
+  </si>
+  <si>
+    <t>digital electronics and microprocessors</t>
+  </si>
+  <si>
+    <t>medical robotics</t>
+  </si>
+  <si>
+    <t>microrobotics</t>
+  </si>
+  <si>
+    <t>operator interface</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>robot locomotion and mobility</t>
+  </si>
+  <si>
+    <t>robot manipulators and effectors</t>
+  </si>
+  <si>
+    <t>sensing and perception</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>digital</t>
+  </si>
+  <si>
+    <t>medic</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>operate</t>
+  </si>
+  <si>
+    <t>programming language</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>effector</t>
+  </si>
+  <si>
+    <t>sensor</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>cybernetics</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>electro</t>
+  </si>
+  <si>
+    <t>surgical</t>
+  </si>
+  <si>
+    <t>miniature</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>mobility</t>
+  </si>
+  <si>
+    <t>kinematic</t>
+  </si>
+  <si>
+    <t>sensing</t>
+  </si>
+  <si>
+    <t>mapping</t>
+  </si>
+  <si>
+    <t>robotic process automation</t>
+  </si>
+  <si>
+    <t>neuro</t>
+  </si>
+  <si>
+    <t>loop</t>
+  </si>
+  <si>
+    <t>micro-processor</t>
+  </si>
+  <si>
+    <t>surgery</t>
+  </si>
+  <si>
+    <t>miniaturization</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>develop</t>
+  </si>
+  <si>
+    <t>motion</t>
+  </si>
+  <si>
+    <t>mechatronic</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>unmanned</t>
+  </si>
+  <si>
+    <t>molecular</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>rehab</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>simulat</t>
+  </si>
+  <si>
+    <t>aero</t>
+  </si>
+  <si>
+    <t>manipulation</t>
+  </si>
+  <si>
+    <t>vision</t>
+  </si>
+  <si>
+    <t>intelligence</t>
+  </si>
+  <si>
+    <t>cellular</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>telepresence</t>
+  </si>
+  <si>
+    <t>swarm</t>
+  </si>
+  <si>
+    <t>teach pendant</t>
+  </si>
+  <si>
+    <t>aerial</t>
+  </si>
+  <si>
+    <t>manipulability</t>
+  </si>
+  <si>
+    <t>avoidance</t>
+  </si>
+  <si>
+    <t>cogni</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>logic</t>
+  </si>
+  <si>
+    <t>pharma</t>
+  </si>
+  <si>
+    <t>mems</t>
+  </si>
+  <si>
+    <t>human-robot</t>
+  </si>
+  <si>
+    <t>off-line</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>dexterous</t>
+  </si>
+  <si>
+    <t>SLAM</t>
+  </si>
+  <si>
+    <t>non-linear</t>
+  </si>
+  <si>
+    <t>companion</t>
+  </si>
+  <si>
+    <t>mini</t>
+  </si>
+  <si>
+    <t>collaboration</t>
+  </si>
+  <si>
+    <t>offline</t>
+  </si>
+  <si>
+    <t>vehicular</t>
+  </si>
+  <si>
+    <t>dexterity</t>
+  </si>
+  <si>
+    <t>Simultaneous localization and mapping</t>
+  </si>
+  <si>
+    <t>decentralised</t>
+  </si>
+  <si>
+    <t>disinfect</t>
+  </si>
+  <si>
+    <t>millirobot</t>
+  </si>
+  <si>
+    <t>collaborative</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>gantry</t>
+  </si>
+  <si>
+    <t>navigation</t>
+  </si>
+  <si>
+    <t>decentralized</t>
+  </si>
+  <si>
+    <t>minimal invasion</t>
+  </si>
+  <si>
+    <t>cobot</t>
+  </si>
+  <si>
+    <t>nautical</t>
+  </si>
+  <si>
+    <t>joint</t>
+  </si>
+  <si>
+    <t>planning</t>
+  </si>
+  <si>
+    <t>deterministic</t>
+  </si>
+  <si>
+    <t>minimally invasive</t>
+  </si>
+  <si>
+    <t>HRI</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>collision</t>
+  </si>
+  <si>
+    <t>stochastic</t>
+  </si>
+  <si>
+    <t>human-robot interaction</t>
+  </si>
+  <si>
+    <t>polar</t>
+  </si>
+  <si>
+    <t>axes</t>
+  </si>
+  <si>
+    <t>signal</t>
+  </si>
+  <si>
+    <t>servo</t>
+  </si>
+  <si>
+    <t>human-robot interface</t>
+  </si>
+  <si>
+    <t>pedal</t>
+  </si>
+  <si>
+    <t>manipulate</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>leg</t>
+  </si>
+  <si>
+    <t>degrees of freedom</t>
+  </si>
+  <si>
+    <t>gesture</t>
+  </si>
+  <si>
+    <t>wheel</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>actuation</t>
+  </si>
+  <si>
+    <t>virtual reality</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>actuator</t>
+  </si>
+  <si>
+    <t>voice control</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>grip</t>
+  </si>
+  <si>
+    <t>haptic</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>drones</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>detect</t>
+  </si>
+  <si>
+    <t>monitoring</t>
+  </si>
+  <si>
+    <t>predictive</t>
+  </si>
+  <si>
+    <t>digitalisation</t>
+  </si>
+  <si>
+    <t>digitilization</t>
+  </si>
+  <si>
+    <t>augmented</t>
+  </si>
+  <si>
+    <t>signalling</t>
+  </si>
+  <si>
+    <t>simulation</t>
+  </si>
+  <si>
+    <t>soft robotics</t>
+  </si>
+  <si>
+    <t>perceptive</t>
+  </si>
+  <si>
+    <t>extracting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -391,9 +953,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -732,25 +1297,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.9140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.25" customWidth="1"/>
-    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -767,7 +1332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -784,7 +1349,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -801,7 +1366,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -818,7 +1383,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -831,6 +1396,9 @@
       <c r="D5" t="s">
         <v>72</v>
       </c>
+      <c r="E5" t="s">
+        <v>287</v>
+      </c>
       <c r="F5" t="s">
         <v>32</v>
       </c>
@@ -838,9 +1406,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
@@ -851,6 +1419,9 @@
       <c r="D6" t="s">
         <v>76</v>
       </c>
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
       <c r="F6" t="s">
         <v>32</v>
       </c>
@@ -858,9 +1429,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
@@ -868,6 +1439,12 @@
       <c r="C7" t="s">
         <v>93</v>
       </c>
+      <c r="D7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
+        <v>290</v>
+      </c>
       <c r="F7" t="s">
         <v>32</v>
       </c>
@@ -875,9 +1452,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -885,6 +1462,12 @@
       <c r="C8" t="s">
         <v>87</v>
       </c>
+      <c r="D8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E8" t="s">
+        <v>167</v>
+      </c>
       <c r="F8" t="s">
         <v>32</v>
       </c>
@@ -892,9 +1475,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -902,6 +1485,12 @@
       <c r="C9" t="s">
         <v>88</v>
       </c>
+      <c r="D9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
       <c r="F9" t="s">
         <v>32</v>
       </c>
@@ -909,9 +1498,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
         <v>80</v>
@@ -919,6 +1508,12 @@
       <c r="C10" t="s">
         <v>89</v>
       </c>
+      <c r="D10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" t="s">
+        <v>257</v>
+      </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
@@ -926,9 +1521,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
@@ -936,8 +1531,11 @@
       <c r="C11" t="s">
         <v>90</v>
       </c>
+      <c r="D11" t="s">
+        <v>265</v>
+      </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>294</v>
       </c>
       <c r="F11" t="s">
         <v>32</v>
@@ -946,10 +1544,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>82</v>
       </c>
@@ -957,10 +1552,10 @@
         <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>295</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>251</v>
       </c>
       <c r="F12" t="s">
         <v>32</v>
@@ -969,7 +1564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -992,7 +1587,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1015,7 +1610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1038,7 +1633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1061,7 +1656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>95</v>
       </c>
@@ -1069,34 +1664,68 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1106,16 +1735,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1138,7 +1767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1161,7 +1790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1184,7 +1813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1230,7 +1859,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1276,7 +1905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1299,7 +1928,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1322,7 +1951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1345,7 +1974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1368,7 +1997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1391,7 +2020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1414,7 +2043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1437,7 +2066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1460,7 +2089,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1489,4 +2118,671 @@
     <ignoredError sqref="A1:G16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="24.8984375" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="16.69921875" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.296875" customWidth="1"/>
+    <col min="7" max="7" width="14.8984375" customWidth="1"/>
+    <col min="8" max="8" width="22.59765625" customWidth="1"/>
+    <col min="9" max="9" width="23.09765625" customWidth="1"/>
+    <col min="10" max="10" width="27.09765625" customWidth="1"/>
+    <col min="11" max="11" width="18.796875" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J3" t="s">
+        <v>183</v>
+      </c>
+      <c r="K3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" t="s">
+        <v>195</v>
+      </c>
+      <c r="K4" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I5" t="s">
+        <v>205</v>
+      </c>
+      <c r="J5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>214</v>
+      </c>
+      <c r="J6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" t="s">
+        <v>224</v>
+      </c>
+      <c r="I7" t="s">
+        <v>225</v>
+      </c>
+      <c r="J7" t="s">
+        <v>226</v>
+      </c>
+      <c r="K7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" t="s">
+        <v>231</v>
+      </c>
+      <c r="H8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J8" t="s">
+        <v>234</v>
+      </c>
+      <c r="K8" t="s">
+        <v>235</v>
+      </c>
+      <c r="L8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" t="s">
+        <v>240</v>
+      </c>
+      <c r="I9" t="s">
+        <v>241</v>
+      </c>
+      <c r="J9" t="s">
+        <v>242</v>
+      </c>
+      <c r="K9" t="s">
+        <v>243</v>
+      </c>
+      <c r="L9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" t="s">
+        <v>248</v>
+      </c>
+      <c r="K10" t="s">
+        <v>249</v>
+      </c>
+      <c r="L10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H11" t="s">
+        <v>253</v>
+      </c>
+      <c r="J11" t="s">
+        <v>254</v>
+      </c>
+      <c r="K11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>257</v>
+      </c>
+      <c r="H12" t="s">
+        <v>258</v>
+      </c>
+      <c r="J12" t="s">
+        <v>259</v>
+      </c>
+      <c r="K12" t="s">
+        <v>260</v>
+      </c>
+      <c r="L12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="H13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J13" t="s">
+        <v>264</v>
+      </c>
+      <c r="K13" t="s">
+        <v>265</v>
+      </c>
+      <c r="L13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>267</v>
+      </c>
+      <c r="J14" t="s">
+        <v>268</v>
+      </c>
+      <c r="K14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>270</v>
+      </c>
+      <c r="J15" t="s">
+        <v>271</v>
+      </c>
+      <c r="K15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" t="s">
+        <v>273</v>
+      </c>
+      <c r="K16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>275</v>
+      </c>
+      <c r="J17" t="s">
+        <v>276</v>
+      </c>
+      <c r="K17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" t="s">
+        <v>279</v>
+      </c>
+      <c r="K18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>281</v>
+      </c>
+      <c r="J19" t="s">
+        <v>186</v>
+      </c>
+      <c r="K19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
second version of keywords.xlsx and change in the color theme for plots
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -1,28 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnandarL\source\repos\SHK-AIRI-Fundamentals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msasafety-my.sharepoint.com/personal/03brandhet37_msasafety_com/Documents/Desktop/HWR/SHK/SHK II/AIRI-Fundamentals/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C14076DD-23F6-4DF5-8F36-6E920DE5CD0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="3108" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="First Draft" sheetId="1" r:id="rId1"/>
-    <sheet name="SchmidtLampe" sheetId="2" r:id="rId2"/>
-    <sheet name="WolfVitale" sheetId="4" r:id="rId3"/>
-    <sheet name="Anandarajah" sheetId="5" r:id="rId4"/>
+    <sheet name="Second Draft" sheetId="6" r:id="rId1"/>
+    <sheet name="First Draft" sheetId="1" r:id="rId2"/>
+    <sheet name="SchmidtLampe" sheetId="2" r:id="rId3"/>
+    <sheet name="WolfVitale" sheetId="4" r:id="rId4"/>
+    <sheet name="Anandarajah" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lemke, Claudia</author>
+  </authors>
+  <commentList>
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{31F797AD-A460-489A-B48A-989FCF7A0F34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lemke, Claudia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+auch hier Überschneidungen zum Thema Technology
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lemke, Claudia</author>
+  </authors>
+  <commentList>
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lemke, Claudia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+auch hier Überschneidungen zum Thema Technology
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="472">
   <si>
     <t>Digitalisierung</t>
   </si>
@@ -910,13 +982,541 @@
   </si>
   <si>
     <t>extracting</t>
+  </si>
+  <si>
+    <t>vorfhersagen</t>
+  </si>
+  <si>
+    <t>wahrnehmen</t>
+  </si>
+  <si>
+    <t>Wahrnehmung</t>
+  </si>
+  <si>
+    <t>maschinelles Lernen</t>
+  </si>
+  <si>
+    <t>Bilderkennung</t>
+  </si>
+  <si>
+    <t>neuronale Netze</t>
+  </si>
+  <si>
+    <t>starke KI</t>
+  </si>
+  <si>
+    <t>schwache KI</t>
+  </si>
+  <si>
+    <t>semantische Analyse</t>
+  </si>
+  <si>
+    <t>natürliche Sprachverarbeitung</t>
+  </si>
+  <si>
+    <t>Computerlinguistik</t>
+  </si>
+  <si>
+    <t>linguistische Datenverarbeitung</t>
+  </si>
+  <si>
+    <t>Spracherkennung</t>
+  </si>
+  <si>
+    <t>syntaktische Analyse</t>
+  </si>
+  <si>
+    <t>Text Mining</t>
+  </si>
+  <si>
+    <t>Informationsextraktion</t>
+  </si>
+  <si>
+    <t>Textverarbeitung</t>
+  </si>
+  <si>
+    <t>Bildverarbeitung</t>
+  </si>
+  <si>
+    <t>Expertensystem</t>
+  </si>
+  <si>
+    <t>Sensorik</t>
+  </si>
+  <si>
+    <t>Robotik</t>
+  </si>
+  <si>
+    <t>cloud computing</t>
+  </si>
+  <si>
+    <t>Mustererkennung</t>
+  </si>
+  <si>
+    <t>Musteranalyse</t>
+  </si>
+  <si>
+    <t>wissensbasierte Systeme</t>
+  </si>
+  <si>
+    <t>Intelligenz</t>
+  </si>
+  <si>
+    <t>Handschrifterkennung</t>
+  </si>
+  <si>
+    <t>Gesichtserkennung</t>
+  </si>
+  <si>
+    <t>Roboter</t>
+  </si>
+  <si>
+    <t>Mustervorhersage</t>
+  </si>
+  <si>
+    <t>Kognition</t>
+  </si>
+  <si>
+    <t>symbolische KI</t>
+  </si>
+  <si>
+    <t>konnektionistische KI</t>
+  </si>
+  <si>
+    <t>Konnektionismus</t>
+  </si>
+  <si>
+    <t>GOFAI</t>
+  </si>
+  <si>
+    <t>neuronale KI</t>
+  </si>
+  <si>
+    <t>Suchalgorithmus</t>
+  </si>
+  <si>
+    <t>Heuristik</t>
+  </si>
+  <si>
+    <t>heuristische Suchverfahren</t>
+  </si>
+  <si>
+    <t>Wissensrepräsentation</t>
+  </si>
+  <si>
+    <t>Beweissysteme</t>
+  </si>
+  <si>
+    <t>Ontologie</t>
+  </si>
+  <si>
+    <t>maschinelle Übersetzung</t>
+  </si>
+  <si>
+    <t>autonomes Fahren</t>
+  </si>
+  <si>
+    <t>autonome Fahrzeuge</t>
+  </si>
+  <si>
+    <t>Texterkennung</t>
+  </si>
+  <si>
+    <t>Zeichenerkennung</t>
+  </si>
+  <si>
+    <t>Computeranimation</t>
+  </si>
+  <si>
+    <t>Computersimulation</t>
+  </si>
+  <si>
+    <t>humanoide Roboter</t>
+  </si>
+  <si>
+    <t>selbstfahrende Kraftfahrzeuge</t>
+  </si>
+  <si>
+    <t>Computerspiele</t>
+  </si>
+  <si>
+    <t>Sprachassistent</t>
+  </si>
+  <si>
+    <t>Sprachverarbeitung</t>
+  </si>
+  <si>
+    <t>virtueller Assistent</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>virtuelle Realität</t>
+  </si>
+  <si>
+    <t>kognitive Systeme</t>
+  </si>
+  <si>
+    <t>virtuelle persönliche Assistenz</t>
+  </si>
+  <si>
+    <t>VPA</t>
+  </si>
+  <si>
+    <t>conversational AI</t>
+  </si>
+  <si>
+    <t>conversational Commerce</t>
+  </si>
+  <si>
+    <t>Dialoghandel</t>
+  </si>
+  <si>
+    <t>automatisierte Assessments</t>
+  </si>
+  <si>
+    <t>Empfehlungssysteme</t>
+  </si>
+  <si>
+    <t>assistive Technologie</t>
+  </si>
+  <si>
+    <t>selbstfahrende Autos</t>
+  </si>
+  <si>
+    <t>Clustering</t>
+  </si>
+  <si>
+    <t>virtual</t>
+  </si>
+  <si>
+    <t>conversational</t>
+  </si>
+  <si>
+    <t>assistiv</t>
+  </si>
+  <si>
+    <t>künstlich</t>
+  </si>
+  <si>
+    <t>semantic</t>
+  </si>
+  <si>
+    <t>semantisch</t>
+  </si>
+  <si>
+    <t>syntactic</t>
+  </si>
+  <si>
+    <t>syntaktisch</t>
+  </si>
+  <si>
+    <t>neuronal</t>
+  </si>
+  <si>
+    <t>neurolale</t>
+  </si>
+  <si>
+    <t>heuristic</t>
+  </si>
+  <si>
+    <t>symbolic</t>
+  </si>
+  <si>
+    <t>autonome</t>
+  </si>
+  <si>
+    <t>linguistic</t>
+  </si>
+  <si>
+    <t>humanoid</t>
+  </si>
+  <si>
+    <t>knowledge-based</t>
+  </si>
+  <si>
+    <t>wissensbasiert</t>
+  </si>
+  <si>
+    <t>sensorisch</t>
+  </si>
+  <si>
+    <t>linguistisch</t>
+  </si>
+  <si>
+    <t>symbolisch</t>
+  </si>
+  <si>
+    <t>heutistisch</t>
+  </si>
+  <si>
+    <t>kognitiv</t>
+  </si>
+  <si>
+    <t>maschinell</t>
+  </si>
+  <si>
+    <t>virtuell</t>
+  </si>
+  <si>
+    <t>selbstfahrend</t>
+  </si>
+  <si>
+    <t>connectionistic</t>
+  </si>
+  <si>
+    <t>konnektionistisch</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>intelligente Fähigkeiten</t>
+  </si>
+  <si>
+    <t>syntactic analysis</t>
+  </si>
+  <si>
+    <t>optical character recognition</t>
+  </si>
+  <si>
+    <t>OCR</t>
+  </si>
+  <si>
+    <t>intelligent character recognition</t>
+  </si>
+  <si>
+    <t>ICR</t>
+  </si>
+  <si>
+    <t>information retrieval</t>
+  </si>
+  <si>
+    <t>Datenanalyse</t>
+  </si>
+  <si>
+    <t>data analysis</t>
+  </si>
+  <si>
+    <t>Classifiers</t>
+  </si>
+  <si>
+    <t>motion detection</t>
+  </si>
+  <si>
+    <t>face recognition</t>
+  </si>
+  <si>
+    <t>pattern recognition</t>
+  </si>
+  <si>
+    <t>speech recognition</t>
+  </si>
+  <si>
+    <t>handwriting recognition</t>
+  </si>
+  <si>
+    <t>image analysis</t>
+  </si>
+  <si>
+    <t>detection</t>
+  </si>
+  <si>
+    <t>prediction</t>
+  </si>
+  <si>
+    <t>Erkennung</t>
+  </si>
+  <si>
+    <t>erkennen</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>intelligent capabilities</t>
+  </si>
+  <si>
+    <t>pattern analysis</t>
+  </si>
+  <si>
+    <t>computational linguistics</t>
+  </si>
+  <si>
+    <t>linguistic data processing</t>
+  </si>
+  <si>
+    <t>Information extraction</t>
+  </si>
+  <si>
+    <t>expert system</t>
+  </si>
+  <si>
+    <t>knowledge representation</t>
+  </si>
+  <si>
+    <t>pattern prediction</t>
+  </si>
+  <si>
+    <t>cognition</t>
+  </si>
+  <si>
+    <t>cognitive systems</t>
+  </si>
+  <si>
+    <t>symbolic AI</t>
+  </si>
+  <si>
+    <t>connectionist AI</t>
+  </si>
+  <si>
+    <t>neural AI</t>
+  </si>
+  <si>
+    <t>connectionism</t>
+  </si>
+  <si>
+    <t>heuristics</t>
+  </si>
+  <si>
+    <t>heuristic search methods</t>
+  </si>
+  <si>
+    <t>ontology</t>
+  </si>
+  <si>
+    <t>machine translation</t>
+  </si>
+  <si>
+    <t>automated assessments</t>
+  </si>
+  <si>
+    <t>recommender systems</t>
+  </si>
+  <si>
+    <t>maschinelle Intelligenz</t>
+  </si>
+  <si>
+    <t>machine intelligence</t>
+  </si>
+  <si>
+    <t>text recognition</t>
+  </si>
+  <si>
+    <t>character recognition</t>
+  </si>
+  <si>
+    <t>handwritten text recognition</t>
+  </si>
+  <si>
+    <t>text processing</t>
+  </si>
+  <si>
+    <t>image processing</t>
+  </si>
+  <si>
+    <t>speech processing</t>
+  </si>
+  <si>
+    <t>knowledge-based systems</t>
+  </si>
+  <si>
+    <t>proof systems</t>
+  </si>
+  <si>
+    <t>search algorithm</t>
+  </si>
+  <si>
+    <t>automatisiert</t>
+  </si>
+  <si>
+    <t>automatic</t>
+  </si>
+  <si>
+    <t>Klassifikationsverfahren</t>
+  </si>
+  <si>
+    <t>visual recognition</t>
+  </si>
+  <si>
+    <t>Es gibt viele Begriffe unter "AI" (Spalte B), die als "AI-Technologien" (Spalte C) gesehen werden, d.h. sie Trennung zwischen Spalten B und C könnte nicht eindeutig sein.</t>
+  </si>
+  <si>
+    <t>entscheiden</t>
+  </si>
+  <si>
+    <t>Entscheidungsvorbereitung</t>
+  </si>
+  <si>
+    <t>Entscheidungsunterstützung</t>
+  </si>
+  <si>
+    <t>Products &amp; Services</t>
+  </si>
+  <si>
+    <t>chat bots</t>
+  </si>
+  <si>
+    <t>Digitale Zwilling</t>
+  </si>
+  <si>
+    <t>Digital Twin</t>
+  </si>
+  <si>
+    <t>hier gibt es wiederrum Überschneidungen zu AI und Technology</t>
+  </si>
+  <si>
+    <t>Facial Recognition</t>
+  </si>
+  <si>
+    <t>Fraud Detection</t>
+  </si>
+  <si>
+    <t>AI-based Software Development</t>
+  </si>
+  <si>
+    <t>cybersecurity/AI-based security</t>
+  </si>
+  <si>
+    <t>etc.</t>
+  </si>
+  <si>
+    <t>z.B. Sprachassistent etc. (siehe Anmerkung oben)</t>
+  </si>
+  <si>
+    <t>assistiertes Fahren</t>
+  </si>
+  <si>
+    <t>ab hier beginnt die Aufzählung einiger Anwendungen auf Basis von KI, wie diese heute als Produkte schon erwerbbar sind - es müssten weitere aufgeführt werden bzw. evtl. eine Entscheidung getroffen werden, ob AI, technology oder Products &amp; Services</t>
+  </si>
+  <si>
+    <t>vorhersagen</t>
+  </si>
+  <si>
+    <t>Product-AI</t>
+  </si>
+  <si>
+    <t>Process-AI</t>
+  </si>
+  <si>
+    <t>cybersecurity security</t>
+  </si>
+  <si>
+    <t>AI-based security</t>
+  </si>
+  <si>
+    <t>AI-Synonyms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -932,13 +1532,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -953,12 +1614,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1297,454 +1970,2270 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183C49BF-D490-4731-BF7B-F9BCD17C2B90}">
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" customWidth="1"/>
-    <col min="5" max="5" width="12.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="27.58203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="24.08203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="10.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>287</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D9" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D10" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E7" t="s">
-        <v>290</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D11" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E9" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>286</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" t="s">
-        <v>170</v>
-      </c>
-      <c r="E10" t="s">
-        <v>257</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>291</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="E25" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E11" t="s">
-        <v>294</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>295</v>
-      </c>
-      <c r="E12" t="s">
-        <v>251</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C18" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" t="s">
-        <v>174</v>
-      </c>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H113"/>
+  <sheetViews>
+    <sheetView topLeftCell="A86" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C99" sqref="A1:H113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="27.75" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="6" max="6" width="35.58203125" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" t="s">
+        <v>281</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B99" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B100" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B101" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B102" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B104" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B105" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B106" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B107" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B108" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B110" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B111" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B112" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B113" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1767,7 +4256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1790,7 +4279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1813,7 +4302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +4325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1859,7 +4348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1882,7 +4371,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1905,7 +4394,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1928,7 +4417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1951,7 +4440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1974,7 +4463,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1997,7 +4486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2020,7 +4509,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2043,7 +4532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2066,7 +4555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2089,7 +4578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2120,17 +4609,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
@@ -2143,12 +4632,12 @@
       <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2160,7 +4649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -2180,7 +4669,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -2200,7 +4689,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -2220,7 +4709,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -2240,7 +4729,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2254,7 +4743,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>126</v>
       </c>
@@ -2265,7 +4754,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>127</v>
       </c>
@@ -2276,7 +4765,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>128</v>
       </c>
@@ -2296,31 +4785,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.8984375" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="16.69921875" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" customWidth="1"/>
-    <col min="6" max="6" width="16.296875" customWidth="1"/>
-    <col min="7" max="7" width="14.8984375" customWidth="1"/>
-    <col min="8" max="8" width="22.59765625" customWidth="1"/>
-    <col min="9" max="9" width="23.09765625" customWidth="1"/>
-    <col min="10" max="10" width="27.09765625" customWidth="1"/>
-    <col min="11" max="11" width="18.796875" customWidth="1"/>
+    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22.58203125" customWidth="1"/>
+    <col min="9" max="9" width="23.08203125" customWidth="1"/>
+    <col min="10" max="10" width="27.08203125" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2358,7 +4846,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2396,7 +4884,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -2434,7 +4922,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -2472,7 +4960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>197</v>
       </c>
@@ -2510,7 +4998,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>209</v>
       </c>
@@ -2545,7 +5033,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -2580,7 +5068,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>229</v>
       </c>
@@ -2606,7 +5094,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>237</v>
       </c>
@@ -2632,7 +5120,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>245</v>
       </c>
@@ -2652,7 +5140,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>251</v>
       </c>
@@ -2672,7 +5160,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>257</v>
       </c>
@@ -2689,7 +5177,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>262</v>
       </c>
@@ -2706,7 +5194,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H14" t="s">
         <v>267</v>
       </c>
@@ -2717,7 +5205,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H15" t="s">
         <v>270</v>
       </c>
@@ -2728,7 +5216,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H16" t="s">
         <v>90</v>
       </c>
@@ -2739,7 +5227,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:11" x14ac:dyDescent="0.35">
       <c r="H17" t="s">
         <v>275</v>
       </c>
@@ -2750,7 +5238,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:11" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
         <v>278</v>
       </c>
@@ -2761,7 +5249,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:11" x14ac:dyDescent="0.35">
       <c r="H19" t="s">
         <v>281</v>
       </c>
@@ -2772,12 +5260,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:11" x14ac:dyDescent="0.35">
       <c r="J20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:11" x14ac:dyDescent="0.35">
       <c r="J21" t="s">
         <v>284</v>
       </c>

</xml_diff>